<commit_message>
pre release for hash code generation.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://simeiosolutions0-my.sharepoint.com/personal/aray_simeio_com/Documents/Documents/UiPath/calculateClientSecurityHash/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E38D392-62AF-4C8A-AC9C-24748BA031EA}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C89FED5-7A62-4E35-85E0-4F8ABADB5F4F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -159,9 +159,6 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
-  </si>
-  <si>
     <t>acmeCred</t>
   </si>
   <si>
@@ -172,6 +169,9 @@
   </si>
   <si>
     <t>https://acme-test.uipath.com/login</t>
+  </si>
+  <si>
+    <t>clientDetails</t>
   </si>
 </sst>
 </file>
@@ -251,8 +251,63 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>228600</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>53340</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1025" name="Control 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1025"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D20136F-A63C-55A3-2045-FF78FAB53B52}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -551,11 +606,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -605,7 +661,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -615,7 +671,6 @@
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="2"/>
       <c r="C3" s="4" t="s">
         <v>32</v>
       </c>
@@ -635,19 +690,19 @@
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
         <v>47</v>
-      </c>
-      <c r="B7" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" t="s">
         <v>45</v>
-      </c>
-      <c r="B9" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1643,6 +1698,35 @@
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <controls>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1025" r:id="rId4" name="Control 1">
+          <controlPr defaultSize="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>228600</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>53340</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1025" r:id="rId4" name="Control 1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </controls>
 </worksheet>
 </file>
 
@@ -2813,8 +2897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
exception screenshot and mail functionality added.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://simeiosolutions0-my.sharepoint.com/personal/aray_simeio_com/Documents/Documents/UiPath/calculateClientSecurityHash/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C89FED5-7A62-4E35-85E0-4F8ABADB5F4F}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67E0768B-02C3-4520-9116-2A0D13995E74}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -270,7 +270,7 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>228600</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>53340</xdr:rowOff>
+          <xdr:rowOff>68580</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -280,7 +280,7 @@
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D20136F-A63C-55A3-2045-FF78FAB53B52}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -308,6 +308,10 @@
     <mc:Fallback/>
   </mc:AlternateContent>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -610,7 +614,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -1716,7 +1720,7 @@
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>228600</xdr:colOff>
                 <xdr:row>2</xdr:row>
-                <xdr:rowOff>53340</xdr:rowOff>
+                <xdr:rowOff>68580</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
@@ -1734,8 +1738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1796,7 +1800,7 @@
         <v>33</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>41</v>

</xml_diff>